<commit_message>
fix(import): prise en charge des numéros de téléphone fix(manage): correction de l'animation
</commit_message>
<xml_diff>
--- a/packages/backend/src/_static/usagers-import-test/import_ok_2.xlsx
+++ b/packages/backend/src/_static/usagers-import-test/import_ok_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/backend/src/ressources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/_static/usagers-import-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDADC8C6-95EF-404F-BB53-2EEF740BCBF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9D52DE-FA1F-054A-9541-6958ADD18F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="159">
   <si>
     <t>Civilité</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Bouaké, Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t>0142424242</t>
   </si>
   <si>
     <t>domicilie2@yopmail.com</t>
@@ -732,9 +729,6 @@
     <t>Amiens</t>
   </si>
   <si>
-    <t>0101010101</t>
-  </si>
-  <si>
     <t>12/12/1999</t>
   </si>
   <si>
@@ -752,11 +746,17 @@
   <si>
     <t>27/02/2018</t>
   </si>
+  <si>
+    <t>dom3@yopmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0#&quot; &quot;##&quot; &quot;##&quot; &quot;##&quot; &quot;##"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1068,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1181,6 +1181,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2942,9 +2949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2984,7 +2991,7 @@
   <sheetData>
     <row r="1" spans="1:49" s="19" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -3014,10 +3021,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -3026,31 +3033,31 @@
         <v>10</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="T1" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>135</v>
-      </c>
       <c r="W1" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X1" s="16" t="s">
         <v>12</v>
@@ -3059,28 +3066,28 @@
         <v>13</v>
       </c>
       <c r="Z1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="AC1" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AE1" s="16" t="s">
         <v>14</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AH1" s="16" t="s">
         <v>15</v>
@@ -3133,16 +3140,16 @@
     </row>
     <row r="2" spans="1:49" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
@@ -3166,53 +3173,53 @@
         <v>37</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>38</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="V2" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="T2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="22" t="s">
+      <c r="W2" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="W2" s="22" t="s">
-        <v>106</v>
       </c>
       <c r="X2" s="21" t="s">
         <v>39</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z2" s="24"/>
       <c r="AA2" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="24"/>
       <c r="AC2" s="24"/>
       <c r="AD2" s="24"/>
       <c r="AE2" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF2" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AG2" s="22"/>
       <c r="AH2" s="22" t="s">
@@ -3250,16 +3257,16 @@
     </row>
     <row r="3" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="21" t="s">
@@ -3268,11 +3275,11 @@
       <c r="G3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>50</v>
+      <c r="H3" s="41">
+        <v>142424242</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>36</v>
@@ -3280,69 +3287,69 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="M3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="Q3" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="R3" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="X3" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="T3" s="21" t="s">
+      <c r="Y3" s="24" t="s">
         <v>94</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="W3" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>95</v>
       </c>
       <c r="Z3" s="24"/>
       <c r="AA3" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB3" s="22"/>
       <c r="AC3" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD3" s="22"/>
       <c r="AE3" s="21"/>
       <c r="AF3" s="22"/>
       <c r="AG3" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AH3" s="22" t="s">
         <v>47</v>
       </c>
       <c r="AI3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AJ3" s="22" t="s">
+      <c r="AK3" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="AL3" s="22"/>
       <c r="AM3" s="22"/>
@@ -3359,43 +3366,45 @@
     </row>
     <row r="4" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>124</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="21"/>
+      <c r="I4" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="37"/>
@@ -3403,37 +3412,37 @@
       <c r="S4" s="22"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y4" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB4" s="22"/>
       <c r="AC4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AD4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF4" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="AE4" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF4" s="22" t="s">
+      <c r="AG4" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="AG4" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
@@ -3454,57 +3463,57 @@
     </row>
     <row r="5" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>152</v>
+      <c r="H5" s="40">
+        <v>609090909</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K5" s="21"/>
       <c r="L5" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N5" s="21" t="s">
         <v>38</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V5" s="22"/>
       <c r="W5" s="22"/>
@@ -3516,11 +3525,11 @@
       <c r="AC5" s="22"/>
       <c r="AD5" s="22"/>
       <c r="AE5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF5" s="22"/>
       <c r="AG5" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH5" s="22"/>
       <c r="AI5" s="22"/>
@@ -3548,7 +3557,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="29"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
@@ -54351,34 +54360,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -54395,82 +54404,82 @@
         <v>43</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>76</v>
-      </c>
       <c r="H2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="H3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -54478,69 +54487,69 @@
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -54548,10 +54557,10 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -54564,7 +54573,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" s="9"/>
     </row>

</xml_diff>

<commit_message>
Mise en production 2.4  (#1372)
* fix: colonnes et tuto

* fix(news): nouveuatés

* fix(interactions): correction mineurs sur l'affichage
fix(chore): suppression de modules inutiles

* fix(custom-docs): correction de la date affichée dans la radiation + mise à jour des tests

* fix(tests): correction des tests de date sur l'import

* fix(import): prise en charge des formats de texte enrichis
fix(facteur): suppression de l'affichage de la procu pour le facteur

* fix(tests): correction de tests plantés

* fix(import): prise en charge des numéros de téléphone
fix(manage): correction de l'animation

* fix(delete): unused file
</commit_message>
<xml_diff>
--- a/packages/backend/src/_static/usagers-import-test/import_ok_2.xlsx
+++ b/packages/backend/src/_static/usagers-import-test/import_ok_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/backend/src/ressources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/_static/usagers-import-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDADC8C6-95EF-404F-BB53-2EEF740BCBF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9D52DE-FA1F-054A-9541-6958ADD18F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="159">
   <si>
     <t>Civilité</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Bouaké, Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t>0142424242</t>
   </si>
   <si>
     <t>domicilie2@yopmail.com</t>
@@ -732,9 +729,6 @@
     <t>Amiens</t>
   </si>
   <si>
-    <t>0101010101</t>
-  </si>
-  <si>
     <t>12/12/1999</t>
   </si>
   <si>
@@ -752,11 +746,17 @@
   <si>
     <t>27/02/2018</t>
   </si>
+  <si>
+    <t>dom3@yopmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0#&quot; &quot;##&quot; &quot;##&quot; &quot;##&quot; &quot;##"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1068,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1181,6 +1181,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2942,9 +2949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2984,7 +2991,7 @@
   <sheetData>
     <row r="1" spans="1:49" s="19" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -3014,10 +3021,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -3026,31 +3033,31 @@
         <v>10</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="T1" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>135</v>
-      </c>
       <c r="W1" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X1" s="16" t="s">
         <v>12</v>
@@ -3059,28 +3066,28 @@
         <v>13</v>
       </c>
       <c r="Z1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB1" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="AC1" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AE1" s="16" t="s">
         <v>14</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AG1" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AH1" s="16" t="s">
         <v>15</v>
@@ -3133,16 +3140,16 @@
     </row>
     <row r="2" spans="1:49" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
@@ -3166,53 +3173,53 @@
         <v>37</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>38</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="V2" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="T2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="22" t="s">
+      <c r="W2" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="W2" s="22" t="s">
-        <v>106</v>
       </c>
       <c r="X2" s="21" t="s">
         <v>39</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z2" s="24"/>
       <c r="AA2" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="24"/>
       <c r="AC2" s="24"/>
       <c r="AD2" s="24"/>
       <c r="AE2" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF2" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AG2" s="22"/>
       <c r="AH2" s="22" t="s">
@@ -3250,16 +3257,16 @@
     </row>
     <row r="3" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="21" t="s">
@@ -3268,11 +3275,11 @@
       <c r="G3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>50</v>
+      <c r="H3" s="41">
+        <v>142424242</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>36</v>
@@ -3280,69 +3287,69 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="M3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="Q3" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="R3" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="X3" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="T3" s="21" t="s">
+      <c r="Y3" s="24" t="s">
         <v>94</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="W3" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>95</v>
       </c>
       <c r="Z3" s="24"/>
       <c r="AA3" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB3" s="22"/>
       <c r="AC3" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD3" s="22"/>
       <c r="AE3" s="21"/>
       <c r="AF3" s="22"/>
       <c r="AG3" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AH3" s="22" t="s">
         <v>47</v>
       </c>
       <c r="AI3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AJ3" s="22" t="s">
+      <c r="AK3" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="AL3" s="22"/>
       <c r="AM3" s="22"/>
@@ -3359,43 +3366,45 @@
     </row>
     <row r="4" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>124</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="21"/>
+      <c r="I4" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="37"/>
@@ -3403,37 +3412,37 @@
       <c r="S4" s="22"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y4" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB4" s="22"/>
       <c r="AC4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AD4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF4" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="AE4" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF4" s="22" t="s">
+      <c r="AG4" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="AG4" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
@@ -3454,57 +3463,57 @@
     </row>
     <row r="5" spans="1:49" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>152</v>
+      <c r="H5" s="40">
+        <v>609090909</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K5" s="21"/>
       <c r="L5" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N5" s="21" t="s">
         <v>38</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V5" s="22"/>
       <c r="W5" s="22"/>
@@ -3516,11 +3525,11 @@
       <c r="AC5" s="22"/>
       <c r="AD5" s="22"/>
       <c r="AE5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF5" s="22"/>
       <c r="AG5" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH5" s="22"/>
       <c r="AI5" s="22"/>
@@ -3548,7 +3557,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="29"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
@@ -54351,34 +54360,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -54395,82 +54404,82 @@
         <v>43</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>76</v>
-      </c>
       <c r="H2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="H3" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -54478,69 +54487,69 @@
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -54548,10 +54557,10 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="9"/>
     </row>
@@ -54564,7 +54573,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" s="9"/>
     </row>

</xml_diff>